<commit_message>
creature team config file
</commit_message>
<xml_diff>
--- a/plan/excel/creature_怪物表.xlsx
+++ b/plan/excel/creature_怪物表.xlsx
@@ -733,7 +733,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -874,7 +874,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5">
-        <v>2001001</v>
+        <v>10001</v>
       </c>
       <c r="B5" t="s">
         <v>27</v>
@@ -906,7 +906,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6">
-        <v>2001002</v>
+        <v>10002</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>28</v>
@@ -915,7 +915,7 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>120</v>
@@ -938,7 +938,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7">
-        <v>2001003</v>
+        <v>10003</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>29</v>
@@ -947,7 +947,7 @@
         <v>3</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>140</v>
@@ -970,7 +970,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8">
-        <v>2001004</v>
+        <v>10004</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>30</v>
@@ -979,7 +979,7 @@
         <v>4</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>160</v>
@@ -1002,7 +1002,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9">
-        <v>2001005</v>
+        <v>10005</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>31</v>
@@ -1011,7 +1011,7 @@
         <v>5</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>180</v>
@@ -1034,7 +1034,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10">
-        <v>2001006</v>
+        <v>10006</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>32</v>
@@ -1043,7 +1043,7 @@
         <v>6</v>
       </c>
       <c r="D10">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>200</v>
@@ -1066,7 +1066,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11">
-        <v>2001007</v>
+        <v>10007</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>33</v>
@@ -1075,7 +1075,7 @@
         <v>7</v>
       </c>
       <c r="D11">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <v>220</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12">
-        <v>2001008</v>
+        <v>10008</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>34</v>
@@ -1107,7 +1107,7 @@
         <v>8</v>
       </c>
       <c r="D12">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <v>240</v>
@@ -1130,7 +1130,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13">
-        <v>2001009</v>
+        <v>10009</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>35</v>
@@ -1139,7 +1139,7 @@
         <v>9</v>
       </c>
       <c r="D13">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <v>260</v>
@@ -1162,7 +1162,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>2001010</v>
+        <v>10010</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>36</v>
@@ -1171,7 +1171,7 @@
         <v>10</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>280</v>
@@ -1194,7 +1194,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>2001011</v>
+        <v>10011</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>37</v>
@@ -1203,7 +1203,7 @@
         <v>11</v>
       </c>
       <c r="D15">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>300</v>
@@ -1226,7 +1226,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>2001012</v>
+        <v>10012</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>38</v>
@@ -1235,7 +1235,7 @@
         <v>12</v>
       </c>
       <c r="D16">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <v>320</v>

</xml_diff>

<commit_message>
add common skill for unit
</commit_message>
<xml_diff>
--- a/plan/excel/creature_怪物表.xlsx
+++ b/plan/excel/creature_怪物表.xlsx
@@ -10,7 +10,7 @@
     <sheet name="CreatureProto" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CreatureProto!$A$1:$L$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CreatureProto!$A$1:$N$4</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -22,7 +22,33 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+每分钟攻击多少次</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -98,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
   <si>
     <t>英雄ID</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -342,10 +368,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>skill#id_lv</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>1001_1|1001_2</t>
   </si>
   <si>
@@ -368,10 +390,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>自带技能</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>aura#id_lv</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -392,6 +410,33 @@
   </si>
   <si>
     <t>2003_1|2003_2</t>
+  </si>
+  <si>
+    <t>攻速</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>特殊技能</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>普通技能</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_extra#id_lv</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_common#id_lv</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>1001_1</t>
+  </si>
+  <si>
+    <t>1001_1</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -789,11 +834,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q10" sqref="Q10"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -801,11 +846,14 @@
     <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5" customWidth="1"/>
-    <col min="5" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -819,31 +867,37 @@
         <v>15</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -857,31 +911,37 @@
         <v>16</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -895,31 +955,37 @@
         <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -933,16 +999,16 @@
         <v>18</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>2</v>
+      <c r="G4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>2</v>
@@ -956,8 +1022,14 @@
       <c r="L4" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="M4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>10001</v>
       </c>
@@ -970,32 +1042,38 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>42</v>
+      <c r="E5" s="3">
+        <v>20</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5">
+        <v>60</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5">
         <v>100</v>
       </c>
-      <c r="H5" s="2">
-        <v>80</v>
-      </c>
-      <c r="I5" s="4">
-        <v>1000</v>
-      </c>
-      <c r="J5" s="4">
+      <c r="J5" s="2">
+        <v>20</v>
+      </c>
+      <c r="K5" s="4">
+        <v>240</v>
+      </c>
+      <c r="L5" s="4">
         <v>6</v>
       </c>
-      <c r="K5" s="4">
+      <c r="M5" s="4">
         <v>5</v>
       </c>
-      <c r="L5" s="4">
+      <c r="N5" s="4">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>10002</v>
       </c>
@@ -1008,32 +1086,38 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="3">
+        <v>22</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6">
+        <v>120</v>
+      </c>
+      <c r="J6" s="2">
+        <v>22</v>
+      </c>
+      <c r="K6" s="4">
+        <v>250</v>
+      </c>
+      <c r="L6" s="4">
+        <v>8</v>
+      </c>
+      <c r="M6" s="4">
+        <v>6</v>
+      </c>
+      <c r="N6" s="4">
         <v>42</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6">
-        <v>120</v>
-      </c>
-      <c r="H6" s="2">
-        <v>90</v>
-      </c>
-      <c r="I6" s="4">
-        <v>1100</v>
-      </c>
-      <c r="J6" s="4">
-        <v>8</v>
-      </c>
-      <c r="K6" s="4">
-        <v>5</v>
-      </c>
-      <c r="L6" s="4">
-        <v>45</v>
-      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>10003</v>
       </c>
@@ -1046,32 +1130,38 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>43</v>
+      <c r="E7" s="3">
+        <v>24</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7">
+        <v>60</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7">
         <v>140</v>
       </c>
-      <c r="H7" s="2">
-        <v>100</v>
-      </c>
-      <c r="I7" s="4">
-        <v>1200</v>
-      </c>
-      <c r="J7" s="4">
+      <c r="J7" s="2">
+        <v>24</v>
+      </c>
+      <c r="K7" s="4">
+        <v>260</v>
+      </c>
+      <c r="L7" s="4">
         <v>10</v>
       </c>
-      <c r="K7" s="4">
-        <v>5</v>
-      </c>
-      <c r="L7" s="4">
-        <v>50</v>
+      <c r="M7" s="4">
+        <v>7</v>
+      </c>
+      <c r="N7" s="4">
+        <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>10004</v>
       </c>
@@ -1084,32 +1174,38 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>43</v>
+      <c r="E8" s="3">
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8">
+        <v>60</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8">
         <v>160</v>
       </c>
-      <c r="H8" s="2">
-        <v>110</v>
-      </c>
-      <c r="I8" s="4">
-        <v>1300</v>
-      </c>
-      <c r="J8" s="4">
+      <c r="J8" s="2">
+        <v>26</v>
+      </c>
+      <c r="K8" s="4">
+        <v>270</v>
+      </c>
+      <c r="L8" s="4">
         <v>12</v>
       </c>
-      <c r="K8" s="4">
-        <v>5</v>
-      </c>
-      <c r="L8" s="4">
-        <v>55</v>
+      <c r="M8" s="4">
+        <v>8</v>
+      </c>
+      <c r="N8" s="4">
+        <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>10005</v>
       </c>
@@ -1122,32 +1218,38 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>44</v>
+      <c r="E9" s="3">
+        <v>28</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9">
+        <v>60</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9">
         <v>180</v>
       </c>
-      <c r="H9" s="2">
-        <v>120</v>
-      </c>
-      <c r="I9" s="4">
-        <v>1400</v>
-      </c>
-      <c r="J9" s="4">
+      <c r="J9" s="2">
+        <v>28</v>
+      </c>
+      <c r="K9" s="4">
+        <v>280</v>
+      </c>
+      <c r="L9" s="4">
         <v>14</v>
       </c>
-      <c r="K9" s="4">
-        <v>5</v>
-      </c>
-      <c r="L9" s="4">
-        <v>60</v>
+      <c r="M9" s="4">
+        <v>9</v>
+      </c>
+      <c r="N9" s="4">
+        <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>10006</v>
       </c>
@@ -1160,32 +1262,38 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>44</v>
+      <c r="E10" s="3">
+        <v>30</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10">
+        <v>60</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10">
         <v>200</v>
       </c>
-      <c r="H10" s="2">
-        <v>130</v>
-      </c>
-      <c r="I10" s="4">
-        <v>1500</v>
-      </c>
-      <c r="J10" s="4">
+      <c r="J10" s="2">
+        <v>30</v>
+      </c>
+      <c r="K10" s="4">
+        <v>290</v>
+      </c>
+      <c r="L10" s="4">
         <v>16</v>
       </c>
-      <c r="K10" s="4">
-        <v>5</v>
-      </c>
-      <c r="L10" s="4">
-        <v>65</v>
+      <c r="M10" s="4">
+        <v>10</v>
+      </c>
+      <c r="N10" s="4">
+        <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10007</v>
       </c>
@@ -1198,32 +1306,38 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>45</v>
+      <c r="E11" s="3">
+        <v>32</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11">
+        <v>60</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11">
         <v>220</v>
       </c>
-      <c r="H11" s="2">
-        <v>140</v>
-      </c>
-      <c r="I11" s="4">
-        <v>1600</v>
-      </c>
-      <c r="J11" s="4">
+      <c r="J11" s="2">
+        <v>32</v>
+      </c>
+      <c r="K11" s="4">
+        <v>300</v>
+      </c>
+      <c r="L11" s="4">
         <v>18</v>
       </c>
-      <c r="K11" s="4">
-        <v>5</v>
-      </c>
-      <c r="L11" s="4">
-        <v>70</v>
+      <c r="M11" s="4">
+        <v>11</v>
+      </c>
+      <c r="N11" s="4">
+        <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>10008</v>
       </c>
@@ -1236,32 +1350,38 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>45</v>
+      <c r="E12" s="3">
+        <v>34</v>
       </c>
       <c r="F12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12">
+        <v>240</v>
+      </c>
+      <c r="J12" s="2">
+        <v>34</v>
+      </c>
+      <c r="K12" s="4">
+        <v>310</v>
+      </c>
+      <c r="L12" s="4">
+        <v>20</v>
+      </c>
+      <c r="M12" s="4">
+        <v>12</v>
+      </c>
+      <c r="N12" s="4">
         <v>54</v>
       </c>
-      <c r="G12">
-        <v>240</v>
-      </c>
-      <c r="H12" s="2">
-        <v>150</v>
-      </c>
-      <c r="I12" s="4">
-        <v>1700</v>
-      </c>
-      <c r="J12" s="4">
-        <v>20</v>
-      </c>
-      <c r="K12" s="4">
-        <v>5</v>
-      </c>
-      <c r="L12" s="4">
-        <v>75</v>
-      </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>10009</v>
       </c>
@@ -1274,32 +1394,38 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>46</v>
+      <c r="E13" s="3">
+        <v>36</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G13">
+        <v>60</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13">
         <v>260</v>
       </c>
-      <c r="H13" s="2">
-        <v>160</v>
-      </c>
-      <c r="I13" s="4">
-        <v>1800</v>
-      </c>
-      <c r="J13" s="4">
+      <c r="J13" s="2">
+        <v>36</v>
+      </c>
+      <c r="K13" s="4">
+        <v>320</v>
+      </c>
+      <c r="L13" s="4">
         <v>22</v>
       </c>
-      <c r="K13" s="4">
-        <v>5</v>
-      </c>
-      <c r="L13" s="4">
-        <v>80</v>
+      <c r="M13" s="4">
+        <v>13</v>
+      </c>
+      <c r="N13" s="4">
+        <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>10010</v>
       </c>
@@ -1312,32 +1438,38 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>46</v>
+      <c r="E14" s="3">
+        <v>38</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G14">
+        <v>60</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14">
         <v>280</v>
       </c>
-      <c r="H14" s="2">
-        <v>170</v>
-      </c>
-      <c r="I14" s="4">
-        <v>1900</v>
-      </c>
-      <c r="J14" s="4">
+      <c r="J14" s="2">
+        <v>38</v>
+      </c>
+      <c r="K14" s="4">
+        <v>330</v>
+      </c>
+      <c r="L14" s="4">
         <v>24</v>
       </c>
-      <c r="K14" s="4">
-        <v>5</v>
-      </c>
-      <c r="L14" s="4">
-        <v>85</v>
+      <c r="M14" s="4">
+        <v>14</v>
+      </c>
+      <c r="N14" s="4">
+        <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>10011</v>
       </c>
@@ -1350,32 +1482,38 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>47</v>
+      <c r="E15" s="3">
+        <v>40</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G15">
+        <v>60</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15">
         <v>300</v>
       </c>
-      <c r="H15" s="2">
-        <v>180</v>
-      </c>
-      <c r="I15" s="4">
-        <v>2000</v>
-      </c>
-      <c r="J15" s="4">
+      <c r="J15" s="2">
+        <v>40</v>
+      </c>
+      <c r="K15" s="4">
+        <v>340</v>
+      </c>
+      <c r="L15" s="4">
         <v>26</v>
       </c>
-      <c r="K15" s="4">
-        <v>5</v>
-      </c>
-      <c r="L15" s="4">
-        <v>90</v>
+      <c r="M15" s="4">
+        <v>15</v>
+      </c>
+      <c r="N15" s="4">
+        <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>10012</v>
       </c>
@@ -1388,29 +1526,35 @@
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>47</v>
+      <c r="E16" s="3">
+        <v>42</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16">
+        <v>60</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16">
         <v>320</v>
       </c>
-      <c r="H16" s="2">
-        <v>190</v>
-      </c>
-      <c r="I16" s="4">
-        <v>2100</v>
-      </c>
-      <c r="J16" s="4">
+      <c r="J16" s="2">
+        <v>42</v>
+      </c>
+      <c r="K16" s="4">
+        <v>350</v>
+      </c>
+      <c r="L16" s="4">
         <v>28</v>
       </c>
-      <c r="K16" s="4">
-        <v>5</v>
-      </c>
-      <c r="L16" s="4">
-        <v>95</v>
+      <c r="M16" s="4">
+        <v>16</v>
+      </c>
+      <c r="N16" s="4">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* modify creature module name
</commit_message>
<xml_diff>
--- a/plan/excel/creature_怪物表.xlsx
+++ b/plan/excel/creature_怪物表.xlsx
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="74">
   <si>
     <t>英雄ID</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -440,6 +440,167 @@
   </si>
   <si>
     <t>lvbu</t>
+  </si>
+  <si>
+    <t>caocao</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>aopi</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>aoren</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>aqiao</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>iubei</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hangfei</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhugeliang</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>g</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>uojia</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>h</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>uanggai</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>j</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>iaxu</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>j</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ushou</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -841,7 +1002,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1040,7 +1201,7 @@
         <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1083,8 +1244,8 @@
       <c r="B6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
-        <v>62</v>
+      <c r="C6" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1127,8 +1288,8 @@
       <c r="B7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
-        <v>62</v>
+      <c r="C7" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1171,8 +1332,8 @@
       <c r="B8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
-        <v>62</v>
+      <c r="C8" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1215,8 +1376,8 @@
       <c r="B9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
-        <v>62</v>
+      <c r="C9" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1259,8 +1420,8 @@
       <c r="B10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C10" t="s">
-        <v>62</v>
+      <c r="C10" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1303,8 +1464,8 @@
       <c r="B11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
-        <v>62</v>
+      <c r="C11" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1347,8 +1508,8 @@
       <c r="B12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C12" t="s">
-        <v>62</v>
+      <c r="C12" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1391,8 +1552,8 @@
       <c r="B13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C13" t="s">
-        <v>62</v>
+      <c r="C13" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1435,8 +1596,8 @@
       <c r="B14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C14" t="s">
-        <v>62</v>
+      <c r="C14" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1479,8 +1640,8 @@
       <c r="B15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C15" t="s">
-        <v>62</v>
+      <c r="C15" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="D15">
         <v>1</v>

</xml_diff>